<commit_message>
addresses recent comments re: TS and AE
</commit_message>
<xml_diff>
--- a/data/source/AE_imputed.xlsx
+++ b/data/source/AE_imputed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoliva/Documents/GitHub/CTDasRDF/data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2031D2D1-1E5C-614E-9C78-576B0068E1F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25555B82-91EB-6643-9D46-F295F5621CCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25340" yWindow="-15360" windowWidth="23940" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="AE" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26375" uniqueCount="1323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26378" uniqueCount="1325">
   <si>
     <t>STUDYID</t>
   </si>
@@ -3977,19 +3976,25 @@
     <t>AEENTPT</t>
   </si>
   <si>
-    <t>2012-08-01</t>
-  </si>
-  <si>
-    <t>2013-12-09</t>
-  </si>
-  <si>
-    <t>2012-07-07</t>
-  </si>
-  <si>
     <t>CAT1</t>
   </si>
   <si>
     <t>SCAT1</t>
+  </si>
+  <si>
+    <t>2012-08-06</t>
+  </si>
+  <si>
+    <t>2012-08-14</t>
+  </si>
+  <si>
+    <t>AFTER</t>
+  </si>
+  <si>
+    <t>BEFORE</t>
+  </si>
+  <si>
+    <t>2014-01-13</t>
   </si>
 </sst>
 </file>
@@ -4359,8 +4364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY1192"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AW7" sqref="AW7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4601,10 +4606,10 @@
         <v>10001316</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>1256</v>
@@ -4738,10 +4743,10 @@
         <v>10001316</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>1256</v>
@@ -4875,10 +4880,10 @@
         <v>10017977</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>1255</v>
@@ -4968,13 +4973,13 @@
         <v>3</v>
       </c>
       <c r="AW4" s="1">
-        <v>10</v>
-      </c>
-      <c r="AX4" s="1">
-        <v>32</v>
+        <v>-2</v>
+      </c>
+      <c r="AX4" s="1" t="s">
+        <v>1323</v>
       </c>
       <c r="AY4" s="5" t="s">
-        <v>1319</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="5" spans="1:51">
@@ -4988,67 +4993,67 @@
         <v>38</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>1291</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1296</v>
+        <v>1297</v>
       </c>
       <c r="G5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="H5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>1302</v>
+        <v>299</v>
       </c>
       <c r="J5" t="s">
-        <v>540</v>
+        <v>299</v>
       </c>
       <c r="K5" s="1">
-        <v>10003851</v>
+        <v>10015150</v>
       </c>
       <c r="L5" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="M5" s="1">
-        <v>10003677</v>
+        <v>10015150</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="O5" s="1">
-        <v>10000032</v>
+        <v>10015151</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="Q5" s="1">
-        <v>10007521</v>
+        <v>10014982</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>1255</v>
       </c>
       <c r="U5" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="V5" s="1">
-        <v>10007541</v>
+        <v>10040785</v>
       </c>
       <c r="W5" t="s">
-        <v>1231</v>
+        <v>1232</v>
       </c>
       <c r="X5" s="1">
-        <v>10007541</v>
+        <v>10040785</v>
       </c>
       <c r="Y5" t="s">
         <v>1252</v>
@@ -5108,10 +5113,28 @@
         <v>41148</v>
       </c>
       <c r="AR5" s="7">
-        <v>41147</v>
+        <v>41128</v>
+      </c>
+      <c r="AS5" s="7">
+        <v>41151</v>
       </c>
       <c r="AT5">
-        <v>22</v>
+        <v>3</v>
+      </c>
+      <c r="AU5">
+        <v>26</v>
+      </c>
+      <c r="AV5" s="1">
+        <v>24</v>
+      </c>
+      <c r="AW5" s="1">
+        <v>25</v>
+      </c>
+      <c r="AX5" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="AY5" s="5" t="s">
+        <v>1320</v>
       </c>
     </row>
     <row r="6" spans="1:51">
@@ -5125,16 +5148,16 @@
         <v>38</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>1291</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1297</v>
+        <v>1298</v>
       </c>
       <c r="G6" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="H6" t="s">
         <v>299</v>
@@ -5143,16 +5166,16 @@
         <v>299</v>
       </c>
       <c r="J6" t="s">
-        <v>299</v>
+        <v>541</v>
       </c>
       <c r="K6" s="1">
-        <v>10015150</v>
+        <v>10024781</v>
       </c>
       <c r="L6" t="s">
         <v>299</v>
       </c>
       <c r="M6" s="1">
-        <v>10015150</v>
+        <v>10015151</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>1280</v>
@@ -5167,10 +5190,10 @@
         <v>10014982</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>1255</v>
@@ -5179,28 +5202,28 @@
         <v>1232</v>
       </c>
       <c r="V6" s="1">
-        <v>10040785</v>
+        <v>10040786</v>
       </c>
       <c r="W6" t="s">
         <v>1232</v>
       </c>
       <c r="X6" s="1">
-        <v>10040785</v>
+        <v>10040786</v>
       </c>
       <c r="Y6" t="s">
-        <v>1252</v>
+        <v>1253</v>
       </c>
       <c r="Z6" t="s">
         <v>1255</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>1285</v>
+        <v>1286</v>
       </c>
       <c r="AB6" s="1" t="s">
         <v>1309</v>
       </c>
       <c r="AC6" t="s">
-        <v>1259</v>
+        <v>1257</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>1260</v>
@@ -5239,7 +5262,7 @@
         <v>1255</v>
       </c>
       <c r="AP6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AQ6" s="7">
         <v>41148</v>
@@ -5247,27 +5270,9 @@
       <c r="AR6" s="7">
         <v>41128</v>
       </c>
-      <c r="AS6" s="7">
-        <v>41151</v>
-      </c>
       <c r="AT6">
         <v>3</v>
       </c>
-      <c r="AU6">
-        <v>26</v>
-      </c>
-      <c r="AV6" s="1">
-        <v>24</v>
-      </c>
-      <c r="AW6" s="1">
-        <v>64</v>
-      </c>
-      <c r="AX6" s="1">
-        <v>32</v>
-      </c>
-      <c r="AY6" s="5" t="s">
-        <v>1320</v>
-      </c>
     </row>
     <row r="7" spans="1:51">
       <c r="A7" t="s">
@@ -5280,82 +5285,82 @@
         <v>38</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>1291</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="G7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>299</v>
+        <v>1302</v>
       </c>
       <c r="J7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="K7" s="1">
-        <v>10024781</v>
+        <v>10003851</v>
       </c>
       <c r="L7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M7" s="1">
-        <v>10015151</v>
+        <v>10003677</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>1280</v>
+        <v>1278</v>
       </c>
       <c r="O7" s="1">
-        <v>10015151</v>
+        <v>10000032</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>1281</v>
+        <v>1279</v>
       </c>
       <c r="Q7" s="1">
-        <v>10014982</v>
+        <v>10007521</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>1255</v>
       </c>
       <c r="U7" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="V7" s="1">
-        <v>10040786</v>
+        <v>10007541</v>
       </c>
       <c r="W7" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="X7" s="1">
-        <v>10040786</v>
+        <v>10007541</v>
       </c>
       <c r="Y7" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="Z7" t="s">
         <v>1255</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="AB7" s="1" t="s">
         <v>1309</v>
       </c>
       <c r="AC7" t="s">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="AD7" s="1" t="s">
         <v>1260</v>
@@ -5394,16 +5399,16 @@
         <v>1255</v>
       </c>
       <c r="AP7" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AQ7" s="7">
         <v>41148</v>
       </c>
       <c r="AR7" s="7">
-        <v>41128</v>
+        <v>41147</v>
       </c>
       <c r="AT7">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:51">
@@ -5459,10 +5464,10 @@
         <v>10014982</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>1255</v>
@@ -5552,13 +5557,13 @@
         <v>24</v>
       </c>
       <c r="AW8" s="1">
-        <v>64</v>
-      </c>
-      <c r="AX8" s="1">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="AX8" s="1" t="s">
+        <v>1322</v>
       </c>
       <c r="AY8" s="5" t="s">
-        <v>1318</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="9" spans="1:51">
@@ -5614,10 +5619,10 @@
         <v>10001316</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>1256</v>
@@ -5751,10 +5756,10 @@
         <v>10001316</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>1321</v>
+        <v>1318</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>1322</v>
+        <v>1319</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>1256</v>

</xml_diff>

<commit_message>
updated Meddra mini ontology and Corrections
This push now contains all the information needed to generate the pilot SDTM AE Domain.
</commit_message>
<xml_diff>
--- a/data/source/AE_imputed.xlsx
+++ b/data/source/AE_imputed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10206"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoliva/Documents/GitHub/CTDasRDF/data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25555B82-91EB-6643-9D46-F295F5621CCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C05D4A-41CE-5E43-BF7B-D2B6750D44F1}" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25340" yWindow="-15360" windowWidth="23940" windowHeight="9900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25600" yWindow="-18820" windowWidth="25600" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AE" sheetId="1" r:id="rId1"/>
@@ -4364,8 +4364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY1192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AW7" sqref="AW7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -4376,7 +4376,7 @@
     <col min="8" max="8" width="37.6640625" customWidth="1"/>
     <col min="9" max="9" width="11.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="37.83203125" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12" style="1" customWidth="1"/>
     <col min="12" max="12" width="43.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.1640625" style="1" customWidth="1"/>
     <col min="14" max="14" width="36.83203125" style="1" customWidth="1"/>
@@ -5175,7 +5175,7 @@
         <v>299</v>
       </c>
       <c r="M6" s="1">
-        <v>10015151</v>
+        <v>10015150</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>1280</v>
@@ -5449,7 +5449,7 @@
         <v>299</v>
       </c>
       <c r="M8" s="1">
-        <v>10015152</v>
+        <v>10015150</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>1280</v>

</xml_diff>

<commit_message>
changes needed to support external Meddra ontology
and other misc changes/corrections.
</commit_message>
<xml_diff>
--- a/data/source/AE_imputed.xlsx
+++ b/data/source/AE_imputed.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10206"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aoliva/Documents/GitHub/CTDasRDF/data/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C05D4A-41CE-5E43-BF7B-D2B6750D44F1}" xr6:coauthVersionLast="42" xr6:coauthVersionMax="42" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1658B251-C7B5-FD43-A5D2-C5947B3F6FEF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25600" yWindow="-18820" windowWidth="25600" windowHeight="20480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="1200" windowWidth="26380" windowHeight="11080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AE" sheetId="1" r:id="rId1"/>
+    <sheet name="Hierarchy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26378" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26420" uniqueCount="1332">
   <si>
     <t>STUDYID</t>
   </si>
@@ -3995,6 +3996,27 @@
   </si>
   <si>
     <t>2014-01-13</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>PTCD</t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>HLTCD</t>
+  </si>
+  <si>
+    <t>HLGT</t>
+  </si>
+  <si>
+    <t>HLGTCD</t>
+  </si>
+  <si>
+    <t>LLT</t>
   </si>
 </sst>
 </file>
@@ -4004,7 +4026,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4030,13 +4052,25 @@
       <color theme="1"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4051,7 +4085,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -4060,6 +4094,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4364,8 +4402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY1192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -5202,13 +5240,13 @@
         <v>1232</v>
       </c>
       <c r="V6" s="1">
-        <v>10040786</v>
+        <v>10040785</v>
       </c>
       <c r="W6" t="s">
         <v>1232</v>
       </c>
       <c r="X6" s="1">
-        <v>10040786</v>
+        <v>10040785</v>
       </c>
       <c r="Y6" t="s">
         <v>1253</v>
@@ -5476,13 +5514,13 @@
         <v>1232</v>
       </c>
       <c r="V8" s="1">
-        <v>10040787</v>
+        <v>10040785</v>
       </c>
       <c r="W8" t="s">
         <v>1232</v>
       </c>
       <c r="X8" s="1">
-        <v>10040787</v>
+        <v>10040785</v>
       </c>
       <c r="Y8" t="s">
         <v>1252</v>
@@ -104599,6 +104637,346 @@
       <c r="AU1192">
         <v>71</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05168480-6D17-B64C-8D58-147DE1ADDD6B}">
+  <dimension ref="A2:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="2"/>
+    <col min="3" max="3" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>1325</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1327</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1329</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1330</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>537</v>
+      </c>
+      <c r="B3" s="8">
+        <v>10003058</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D3" s="8">
+        <v>10003041</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F3" s="2">
+        <v>10003057</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1275</v>
+      </c>
+      <c r="H3" s="2">
+        <v>10001316</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J3" s="2">
+        <v>10018065</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>295</v>
+      </c>
+      <c r="B4" s="8">
+        <v>10003041</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" t="s">
+        <v>1243</v>
+      </c>
+      <c r="J4" s="2">
+        <v>10022117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="C5" s="2"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F5" s="2">
+        <v>10015151</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10014982</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J5" s="2">
+        <v>10040785</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="C6" s="9"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>538</v>
+      </c>
+      <c r="B7" s="2">
+        <v>10003047</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" s="2">
+        <v>10003053</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1274</v>
+      </c>
+      <c r="F7" s="2">
+        <v>10003057</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1275</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10001316</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>1229</v>
+      </c>
+      <c r="J7" s="2">
+        <v>10018065</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" t="s">
+        <v>1243</v>
+      </c>
+      <c r="J8" s="2">
+        <v>10022117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>539</v>
+      </c>
+      <c r="B10" s="2">
+        <v>10012727</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D10" s="2">
+        <v>10012735</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>1276</v>
+      </c>
+      <c r="F10" s="2">
+        <v>10012736</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1277</v>
+      </c>
+      <c r="H10" s="2">
+        <v>10017977</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>1230</v>
+      </c>
+      <c r="J10" s="2">
+        <v>10017947</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
+        <v>299</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10015150</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D12" s="2">
+        <v>10015150</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10015151</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1281</v>
+      </c>
+      <c r="H12" s="2">
+        <v>10014982</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>1232</v>
+      </c>
+      <c r="J12" s="2">
+        <v>10040785</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>541</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10024781</v>
+      </c>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
+        <v>295</v>
+      </c>
+      <c r="B14" s="8">
+        <v>10003041</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
+        <v>540</v>
+      </c>
+      <c r="B15" s="2">
+        <v>10003851</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D15" s="2">
+        <v>10003677</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1278</v>
+      </c>
+      <c r="F15" s="2">
+        <v>10000032</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="H15" s="2">
+        <v>10007521</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>1231</v>
+      </c>
+      <c r="J15" s="2">
+        <v>10007541</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>